<commit_message>
versão 2 email + Babi imagem
</commit_message>
<xml_diff>
--- a/controle site Helly.xlsx
+++ b/controle site Helly.xlsx
@@ -113,10 +113,10 @@
     <t>Valor combinado R$60,00/hora</t>
   </si>
   <si>
-    <t>Criação de E-mail em HTML - versão 1</t>
-  </si>
-  <si>
-    <t>1h15</t>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>Criação de E-mail em HTML - versão 1 e alterações para 2.</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -638,13 +638,13 @@
         <v>41469</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D3" s="2">
-        <v>1.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -671,7 +671,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5">
         <f>SUM(D3:D7)</f>
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="E8" s="5"/>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="D9" s="2">
         <f>60*D8</f>
-        <v>75</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20.25" x14ac:dyDescent="0.35">

</xml_diff>